<commit_message>
working on revisions, deleting some old files and cleaning up code.
</commit_message>
<xml_diff>
--- a/results/LarvalAbundSensitivity.xlsx
+++ b/results/LarvalAbundSensitivity.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrissy/JointProgram/SlopeSea/2016_data/SlopeSeaBluefinTuna/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A6C4723-244F-B642-9A93-498FA9EFD661}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B2D367-197D-0A47-9749-CA6755363F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39160" yWindow="3920" windowWidth="28040" windowHeight="16940" xr2:uid="{46D85B45-EA6A-BE45-AB93-A408423AB663}"/>
+    <workbookView xWindow="38720" yWindow="4580" windowWidth="28040" windowHeight="16940" xr2:uid="{46D85B45-EA6A-BE45-AB93-A408423AB663}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Configuration</t>
   </si>
@@ -69,19 +69,22 @@
     <t>SEAMAP data 2016, all stations (April 30 to May 30)</t>
   </si>
   <si>
-    <t xml:space="preserve">In the SEAMAP data, 35% of the stations are in water shallower than 1000 m. There are also high catches at some of these shallower stations. </t>
-  </si>
-  <si>
     <t>Bigelow cruise, 31 day window (June 28 to July 28), area stratified mean</t>
   </si>
   <si>
-    <t>Area stratified mean includes shallow stations; Offshore mean = 2.09 (12.05), shelfbreak mean = 0.71 (9.03)</t>
-  </si>
-  <si>
-    <t>Area stratified mean includes shallow stations; Offshore mean = 2.58 (12.05), shelfbreak mean = 1.29 (9.03)</t>
-  </si>
-  <si>
-    <t>Area stratified mean includes shallow stations; Offshore mean = 2.93 (12.05), shelfbreak mean = 0.38 (6.15)</t>
+    <t>Area stratified mean includes shallow stations; Offshore mean = 2.16 (12.49), shelfbreak mean = 1.15 (14.57)</t>
+  </si>
+  <si>
+    <t>Area stratified mean includes shallow stations; Offshore mean = 2.68 (12.49), shelfbreak mean = 2.08 (14.57)</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Area stratified mean includes shallow stations; Offshore mean = 3.04 (12.49), shelfbreak mean = 0.38 (6.15); Can't calculate larval index in this case because there is only 1 station in the shelfbreak region.</t>
+  </si>
+  <si>
+    <t>In the SEAMAP data, 35% of the stations are in water shallower than 1000 m. There are also high catches at some of these shallower stations. I can't calculate larval index because I don't have the lengths of individuals.</t>
   </si>
 </sst>
 </file>
@@ -449,7 +452,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -489,10 +492,13 @@
         <v>60</v>
       </c>
       <c r="C2" s="3">
-        <v>2.54</v>
+        <v>2.79</v>
       </c>
       <c r="D2" s="3">
-        <v>10.71</v>
+        <v>11.75</v>
+      </c>
+      <c r="E2">
+        <v>1.24</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
@@ -506,10 +512,13 @@
         <v>49</v>
       </c>
       <c r="C3" s="3">
-        <v>2.42</v>
+        <v>2.79</v>
       </c>
       <c r="D3" s="3">
-        <v>11.3</v>
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>1.29</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
@@ -523,10 +532,13 @@
         <v>42</v>
       </c>
       <c r="C4" s="3">
-        <v>1.79</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="D4" s="3">
-        <v>10.57</v>
+        <v>12.15</v>
+      </c>
+      <c r="E4">
+        <v>0.94</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>
@@ -540,10 +552,13 @@
         <v>42</v>
       </c>
       <c r="C5" s="3">
-        <v>2.77</v>
+        <v>3.19</v>
       </c>
       <c r="D5" s="3">
-        <v>11.3</v>
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>1.48</v>
       </c>
       <c r="F5" t="s">
         <v>7</v>
@@ -554,16 +569,19 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="C6" s="3">
-        <v>1.79</v>
+        <v>1.94</v>
       </c>
       <c r="D6" s="3">
-        <v>11.4</v>
+        <v>12.94</v>
+      </c>
+      <c r="E6">
+        <v>0.81</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -574,27 +592,33 @@
         <v>42</v>
       </c>
       <c r="C7" s="3">
-        <v>2.2999999999999998</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="D7" s="3">
-        <v>11.4</v>
+        <v>12.94</v>
+      </c>
+      <c r="E7">
+        <v>1.1200000000000001</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>31</v>
       </c>
       <c r="C8" s="3">
-        <v>2.38</v>
+        <v>2.46</v>
       </c>
       <c r="D8" s="3">
-        <v>10.77</v>
+        <v>11.12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
       </c>
       <c r="F8" t="s">
         <v>18</v>
@@ -614,7 +638,7 @@
         <v>38.92</v>
       </c>
       <c r="F9" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>